<commit_message>
Konw how to Switch Sence & Ctrl a Player and Entity
</commit_message>
<xml_diff>
--- a/AAAGameData/DataTables/LevelTable.xlsx
+++ b/AAAGameData/DataTables/LevelTable.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GF_X\AAAGameData\DataTables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity\Fork Project\GF_X_Demo\AAAGameData\DataTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16861C6C-B2B7-4D01-BF98-DCC70084CF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="2775" windowWidth="25860" windowHeight="14685"/>
+    <workbookView xWindow="14220" yWindow="3420" windowWidth="16410" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>#</t>
   </si>
@@ -105,11 +106,19 @@
     <t>i18n</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Lv_0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level.DisplayName6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -163,9 +172,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -440,11 +449,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -614,6 +623,23 @@
         <v>19</v>
       </c>
     </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10">
+        <v>315</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revert "Konw how to Switch Sence & Ctrl a Player and Entity"
This reverts commit e8ffd0b5c8067be177500693721c760003c5ca1c.
</commit_message>
<xml_diff>
--- a/AAAGameData/DataTables/LevelTable.xlsx
+++ b/AAAGameData/DataTables/LevelTable.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity\Fork Project\GF_X_Demo\AAAGameData\DataTables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GF_X\AAAGameData\DataTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16861C6C-B2B7-4D01-BF98-DCC70084CF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14220" yWindow="3420" windowWidth="16410" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="2775" windowWidth="25860" windowHeight="14685"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>#</t>
   </si>
@@ -106,19 +105,11 @@
     <t>i18n</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
-  <si>
-    <t>Lv_0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Level.DisplayName6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -172,9 +163,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -449,11 +440,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -623,23 +614,6 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B10">
-        <v>6</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10">
-        <v>315</v>
-      </c>
-      <c r="F10">
-        <v>3</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>